<commit_message>
added new ML model performance plot to Excel spreadsheet
</commit_message>
<xml_diff>
--- a/dev/tables_and_other/ML_model_performance.xlsx
+++ b/dev/tables_and_other/ML_model_performance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phil\Documents\GitHub\point_cloud_vegetation_filtering\dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phil\Documents\GitHub\point_cloud_vegetation_filtering\dev\tables_and_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6454F8F3-8794-4095-9054-A2E0705BA861}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD18F405-8C39-4660-9E4D-9E023C21089E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{8DCF5AFF-D886-48A3-80E0-141B4EF1DBE8}"/>
   </bookViews>
@@ -12327,6 +12327,1315 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>all models</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>analysis_UPDATED_functions!$G$10:$G$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2785</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11169</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44321</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176161</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2849</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11233</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44385</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>176225</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2945</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11329</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44481</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>176321</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>265</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>analysis_UPDATED_functions!$D$10:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.91479999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93910000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93989999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.93979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91569999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93969999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94030000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94059999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94089999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.94099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.93989999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.94040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.94130000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.94220000000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.94169999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.93479999999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.93879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.93940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.94030000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.85650000000000004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.92589999999999995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.92610000000000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.93640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.93940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.93640000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C986-4507-B437-660845EB975E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1124727360"/>
+        <c:axId val="1124727776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1124727360"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124727776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1124727776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124727360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>1-6</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> layer models</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>analysis_UPDATED_functions!$G$10:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2785</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11169</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44321</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176161</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2849</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11233</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44385</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>176225</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2945</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11329</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44481</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>176321</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>analysis_UPDATED_functions!$D$10:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.91479999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93910000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93989999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.93979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91569999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93969999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94030000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94059999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94089999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.94099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.93989999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.94040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.94130000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.94220000000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.94169999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8A3-4578-B055-FEAF4BDD492E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1124727360"/>
+        <c:axId val="1124727776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1124727360"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124727776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1124727776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124727360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>2-3</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> layer models</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>analysis_UPDATED_functions!$G$28:$G$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>265</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>analysis_UPDATED_functions!$D$28:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.93479999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94030000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85650000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92589999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92610000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.93940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.93640000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CD5A-4085-98DD-D29ECFC0A4F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1124727360"/>
+        <c:axId val="1124727776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1124727360"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124727776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1124727776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124727360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Computing Standard Deviation over r=0.5m</a:t>
             </a:r>
           </a:p>
@@ -12783,7 +14092,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -19256,6 +20565,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors27.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors28.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -28825,6 +30254,1554 @@
 </file>
 
 <file path=xl/charts/style26.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style27.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style28.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style29.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -33869,6 +36846,120 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CD332FE-4306-40F7-9AF1-3EFCCB96D4B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24D46858-D0E5-4C70-BCC1-3DDB7C8334D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="18" name="Chart 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDA9C338-9FCE-49AC-9E61-356FF59E2EA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -37107,8 +40198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9EEADE-EB92-49D2-AC21-19FD28E12729}">
   <dimension ref="A1:AP43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>